<commit_message>
Update application with latest changes
</commit_message>
<xml_diff>
--- a/uploads/question_bulk_import_template.xlsx
+++ b/uploads/question_bulk_import_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{555A6AF6-05BB-42F9-BABF-047AB2853E51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8076092-29F4-43D6-8B1F-20D599560C1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t>Question Text</t>
   </si>
@@ -82,9 +82,6 @@
     <t>true_false</t>
   </si>
   <si>
-    <t>True</t>
-  </si>
-  <si>
     <t>Scientific evidence confirms the Earth is an oblate spheroid.</t>
   </si>
   <si>
@@ -92,9 +89,6 @@
   </si>
   <si>
     <t>short_answer</t>
-  </si>
-  <si>
-    <t>4</t>
   </si>
   <si>
     <t>Basic arithmetic: 2 + 2 = 4.</t>
@@ -475,7 +469,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,54 +545,54 @@
       <c r="B3" t="s">
         <v>19</v>
       </c>
-      <c r="G3" t="s">
-        <v>20</v>
+      <c r="G3" t="b">
+        <v>1</v>
       </c>
       <c r="H3" t="s">
         <v>16</v>
       </c>
       <c r="I3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
         <v>22</v>
       </c>
-      <c r="B4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" t="s">
-        <v>24</v>
+      <c r="G4">
+        <v>4</v>
       </c>
       <c r="H4" t="s">
         <v>16</v>
       </c>
       <c r="I4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
       <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s">
         <v>27</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>28</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>29</v>
-      </c>
-      <c r="F5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G5" t="s">
-        <v>31</v>
       </c>
       <c r="H5" t="s">
         <v>16</v>
@@ -606,13 +600,13 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
         <v>19</v>
       </c>
-      <c r="G6" t="s">
-        <v>20</v>
+      <c r="G6" t="b">
+        <v>1</v>
       </c>
       <c r="H6" t="s">
         <v>16</v>

</xml_diff>